<commit_message>
add missing coords for middle keys surveys from FWC, cluster sites ~1km apart
</commit_message>
<xml_diff>
--- a/FL_APAL_Summary Data.xlsx
+++ b/FL_APAL_Summary Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcunning/Projects/FL_Acropora_2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosscunning/Projects/FLAcro23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95BE70E-000F-6C42-8BF1-1096BA4037E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CEDD88-7CA6-924B-A6C6-CAFE0FFA0923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="9200" windowWidth="23260" windowHeight="9620" activeTab="1" xr2:uid="{17F73F63-56F7-4021-BD24-604BFB2BB2B9}"/>
+    <workbookView xWindow="13560" yWindow="3180" windowWidth="23260" windowHeight="15820" xr2:uid="{17F73F63-56F7-4021-BD24-604BFB2BB2B9}"/>
   </bookViews>
   <sheets>
     <sheet name="FWC" sheetId="1" r:id="rId1"/>
@@ -950,7 +950,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1111,11 +1111,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1433,8 +1428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15B9429-CEB4-4B08-9EA4-931A3271A551}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1738,6 +1733,12 @@
       <c r="D6" t="s">
         <v>30</v>
       </c>
+      <c r="E6" s="1">
+        <v>24.546469999999999</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-81.405529999999999</v>
+      </c>
       <c r="G6" t="s">
         <v>21</v>
       </c>
@@ -1782,6 +1783,12 @@
       <c r="D7" t="s">
         <v>30</v>
       </c>
+      <c r="E7" s="1">
+        <v>24.546469999999999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-81.405529999999999</v>
+      </c>
       <c r="G7" t="s">
         <v>21</v>
       </c>
@@ -1829,8 +1836,12 @@
       <c r="D8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="E8" s="1">
+        <v>24.546469999999999</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-81.405529999999999</v>
+      </c>
       <c r="G8" s="12" t="s">
         <v>21</v>
       </c>
@@ -1879,6 +1890,12 @@
       <c r="D9" t="s">
         <v>30</v>
       </c>
+      <c r="E9" s="1">
+        <v>24.546469999999999</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-81.405529999999999</v>
+      </c>
       <c r="G9" t="s">
         <v>21</v>
       </c>
@@ -1920,6 +1937,12 @@
       <c r="D10" t="s">
         <v>30</v>
       </c>
+      <c r="E10" s="1">
+        <v>24.546469999999999</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-81.405529999999999</v>
+      </c>
       <c r="G10" t="s">
         <v>21</v>
       </c>
@@ -1965,8 +1988,12 @@
       <c r="D11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="E11" s="1">
+        <v>24.546469999999999</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-81.405529999999999</v>
+      </c>
       <c r="G11" s="12" t="s">
         <v>21</v>
       </c>
@@ -2095,6 +2122,12 @@
       <c r="D14" t="s">
         <v>30</v>
       </c>
+      <c r="E14" s="1">
+        <v>24.626159999999999</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-81.110600000000005</v>
+      </c>
       <c r="G14" t="s">
         <v>23</v>
       </c>
@@ -2136,6 +2169,12 @@
       <c r="D15" t="s">
         <v>30</v>
       </c>
+      <c r="E15" s="1">
+        <v>24.626159999999999</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-81.110600000000005</v>
+      </c>
       <c r="G15" t="s">
         <v>23</v>
       </c>
@@ -2183,8 +2222,12 @@
       <c r="D16" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="E16" s="1">
+        <v>24.626159999999999</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-81.110600000000005</v>
+      </c>
       <c r="G16" s="12" t="s">
         <v>23</v>
       </c>
@@ -2233,6 +2276,12 @@
       <c r="D17" t="s">
         <v>30</v>
       </c>
+      <c r="E17" s="1">
+        <v>24.626159999999999</v>
+      </c>
+      <c r="F17" s="1">
+        <v>-81.110600000000005</v>
+      </c>
       <c r="G17" t="s">
         <v>23</v>
       </c>
@@ -2271,6 +2320,12 @@
       <c r="D18" t="s">
         <v>30</v>
       </c>
+      <c r="E18" s="1">
+        <v>24.626159999999999</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-81.110600000000005</v>
+      </c>
       <c r="G18" t="s">
         <v>23</v>
       </c>
@@ -2316,8 +2371,12 @@
       <c r="D19" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="E19" s="1">
+        <v>24.626159999999999</v>
+      </c>
+      <c r="F19" s="1">
+        <v>-81.110600000000005</v>
+      </c>
       <c r="G19" s="12" t="s">
         <v>23</v>
       </c>
@@ -2496,6 +2555,12 @@
       <c r="D23" t="s">
         <v>30</v>
       </c>
+      <c r="E23" s="98">
+        <v>25.316179999999999</v>
+      </c>
+      <c r="F23" s="98">
+        <v>-80.187916000000001</v>
+      </c>
       <c r="G23" t="s">
         <v>25</v>
       </c>
@@ -2537,8 +2602,12 @@
       <c r="D24" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="E24" s="98">
+        <v>25.316179999999999</v>
+      </c>
+      <c r="F24" s="98">
+        <v>-80.187916000000001</v>
+      </c>
       <c r="G24" s="12" t="s">
         <v>25</v>
       </c>
@@ -2635,6 +2704,12 @@
       <c r="D26" t="s">
         <v>30</v>
       </c>
+      <c r="E26" s="98">
+        <v>25.373200000000001</v>
+      </c>
+      <c r="F26" s="98">
+        <v>-80.160309999999996</v>
+      </c>
       <c r="G26" t="s">
         <v>25</v>
       </c>
@@ -2675,8 +2750,12 @@
       <c r="D27" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
+      <c r="E27" s="98">
+        <v>25.373200000000001</v>
+      </c>
+      <c r="F27" s="98">
+        <v>-80.160309999999996</v>
+      </c>
       <c r="G27" s="12" t="s">
         <v>25</v>
       </c>
@@ -2778,7 +2857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A75094-8F95-4D6C-9717-7428BB8597D3}">
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -2919,10 +2998,10 @@
       <c r="A3" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="104" t="s">
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="104" t="s">
+      <c r="C3" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -2934,39 +3013,31 @@
       <c r="F3" s="12">
         <v>-80.140879999999996</v>
       </c>
-      <c r="G3" s="106" t="s">
+      <c r="G3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="105">
+      <c r="H3" s="54">
         <v>45156</v>
       </c>
-      <c r="I3" s="104">
-        <v>100</v>
-      </c>
-      <c r="J3" s="104">
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3">
         <v>10</v>
       </c>
-      <c r="K3" s="106">
-        <v>0</v>
-      </c>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
-      <c r="Q3" s="104"/>
-      <c r="R3" s="104"/>
-      <c r="S3" s="104"/>
+      <c r="K3">
+        <v>0</v>
+      </c>
       <c r="T3" s="50"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="104" t="s">
+      <c r="C4" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -2978,29 +3049,21 @@
       <c r="F4" s="12">
         <v>-80.184259999999995</v>
       </c>
-      <c r="G4" s="106" t="s">
+      <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="105">
+      <c r="H4" s="54">
         <v>45161</v>
       </c>
-      <c r="I4" s="104">
+      <c r="I4">
         <v>62.5</v>
       </c>
-      <c r="J4" s="104">
+      <c r="J4">
         <v>8</v>
       </c>
-      <c r="K4" s="106">
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-      <c r="N4" s="104"/>
-      <c r="O4" s="104"/>
-      <c r="P4" s="104"/>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="104"/>
-      <c r="S4" s="104"/>
       <c r="T4" s="50"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fill in missing values
</commit_message>
<xml_diff>
--- a/FL_APAL_Summary Data.xlsx
+++ b/FL_APAL_Summary Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosscunning/Projects/FLAcro23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CEDD88-7CA6-924B-A6C6-CAFE0FFA0923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545EE4B1-1D19-2D47-BCFC-C8810AA41645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13560" yWindow="3180" windowWidth="23260" windowHeight="15820" xr2:uid="{17F73F63-56F7-4021-BD24-604BFB2BB2B9}"/>
+    <workbookView xWindow="1500" yWindow="1880" windowWidth="23260" windowHeight="15820" xr2:uid="{17F73F63-56F7-4021-BD24-604BFB2BB2B9}"/>
   </bookViews>
   <sheets>
     <sheet name="FWC" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="171">
   <si>
     <t>Site</t>
   </si>
@@ -1429,7 +1429,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1908,8 +1908,8 @@
       <c r="J9">
         <v>18</v>
       </c>
-      <c r="K9" t="s">
-        <v>32</v>
+      <c r="K9">
+        <v>18</v>
       </c>
       <c r="L9" s="30" t="s">
         <v>32</v>
@@ -2294,8 +2294,8 @@
       <c r="J17">
         <v>22</v>
       </c>
-      <c r="K17" t="s">
-        <v>32</v>
+      <c r="K17">
+        <v>22</v>
       </c>
       <c r="L17" s="30" t="s">
         <v>32</v>
@@ -2765,7 +2765,9 @@
       <c r="I27" s="12">
         <v>100</v>
       </c>
-      <c r="J27" s="12"/>
+      <c r="J27" s="12">
+        <v>14</v>
+      </c>
       <c r="K27" s="12">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
DM corrections to FWC data
</commit_message>
<xml_diff>
--- a/FL_APAL_Summary Data.xlsx
+++ b/FL_APAL_Summary Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosscunning/Projects/FLAcro23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545EE4B1-1D19-2D47-BCFC-C8810AA41645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA6830D-32E5-A346-B900-2BC8D3221F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1880" windowWidth="23260" windowHeight="15820" xr2:uid="{17F73F63-56F7-4021-BD24-604BFB2BB2B9}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="23260" windowHeight="15820" xr2:uid="{17F73F63-56F7-4021-BD24-604BFB2BB2B9}"/>
   </bookViews>
   <sheets>
     <sheet name="FWC" sheetId="1" r:id="rId1"/>
@@ -1429,7 +1429,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1906,10 +1906,10 @@
         <v>32</v>
       </c>
       <c r="J9">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L9" s="30" t="s">
         <v>32</v>
@@ -1954,7 +1954,7 @@
         <v>66.666666666666657</v>
       </c>
       <c r="J10">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="K10">
         <v>12</v>
@@ -2004,7 +2004,7 @@
         <v>100</v>
       </c>
       <c r="J11" s="12">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="K11" s="12">
         <v>0</v>
@@ -2337,7 +2337,7 @@
         <v>63.636363636363633</v>
       </c>
       <c r="J18">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K18">
         <v>14</v>
@@ -2388,7 +2388,7 @@
         <v>77.272727272727266</v>
       </c>
       <c r="J19" s="12">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="K19" s="12">
         <v>5</v>

</xml_diff>